<commit_message>
* Fixes in coulm naming convention.
</commit_message>
<xml_diff>
--- a/tests/data/desired/stricttypessuccess.xlsx
+++ b/tests/data/desired/stricttypessuccess.xlsx
@@ -20,7 +20,7 @@
     <t># of Diffs</t>
   </si>
   <si>
-    <t>1</t>
+    <t>1 / ID</t>
   </si>
   <si>
     <t>FIRST_NAME (Source1)</t>
@@ -219,7 +219,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="14.03515625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="7.2109375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="26.10546875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="26.10546875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="25.59765625" customWidth="true" bestFit="true"/>

</xml_diff>